<commit_message>
Avance validaciones 1 al 10
Se avanza en validaciones del 1 al 10 y se incluye analisis de validacion de reportes y mantenedor
</commit_message>
<xml_diff>
--- a/Analisis/validaciones/validacion_reportes.xlsx
+++ b/Analisis/validaciones/validacion_reportes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/validaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{C3BC911C-CB85-46EA-967D-51D15C7D4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84D96C53-A389-42F6-A3C7-4388E00B6A98}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{C3BC911C-CB85-46EA-967D-51D15C7D4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7176BCD-68CB-4DE5-87C4-7F14F4D4788A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13590" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diccionario_validador" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>num_validador</t>
   </si>
@@ -169,6 +169,30 @@
   </si>
   <si>
     <t>Corresponde a validar el dato que solicita RDC01 para el campo Deuda Acelerada</t>
+  </si>
+  <si>
+    <t>Funcion/Procedimiento</t>
+  </si>
+  <si>
+    <t>proceso.val_num_1</t>
+  </si>
+  <si>
+    <t>proceso.val_num_2</t>
+  </si>
+  <si>
+    <t>proceso.val_num_3</t>
+  </si>
+  <si>
+    <t>proceso.val_num_9</t>
+  </si>
+  <si>
+    <t>proceso.val_num_4</t>
+  </si>
+  <si>
+    <t>proceso.val_codigo_tabla</t>
+  </si>
+  <si>
+    <t>proceso.val_num_10</t>
   </si>
 </sst>
 </file>
@@ -234,6 +258,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,23 +527,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="151.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="76.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="151.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,11 +557,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -545,11 +577,14 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -562,11 +597,14 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -579,11 +617,14 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -596,11 +637,14 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -613,11 +657,14 @@
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -630,11 +677,14 @@
       <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -647,11 +697,14 @@
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -664,11 +717,14 @@
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -681,11 +737,14 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -698,11 +757,14 @@
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -715,11 +777,11 @@
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -732,11 +794,11 @@
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -749,7 +811,7 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avance en Validacion RDC01
Se crean funciones y procedimiento de validacion RDC01
</commit_message>
<xml_diff>
--- a/Analisis/validaciones/validacion_reportes.xlsx
+++ b/Analisis/validaciones/validacion_reportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/validaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{C3BC911C-CB85-46EA-967D-51D15C7D4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7176BCD-68CB-4DE5-87C4-7F14F4D4788A}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="13_ncr:1_{C3BC911C-CB85-46EA-967D-51D15C7D4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{598B92BE-EC3A-4F37-A2D0-6FF2E4D670BF}"/>
   <bookViews>
     <workbookView xWindow="13590" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>num_validador</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>proceso.val_num_10</t>
+  </si>
+  <si>
+    <t>proceso.val_num_11</t>
+  </si>
+  <si>
+    <t>proceso.val_en_dominio</t>
   </si>
 </sst>
 </file>
@@ -530,7 +536,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -777,6 +783,9 @@
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>45</v>
       </c>
@@ -794,6 +803,9 @@
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F13" s="3" t="s">
         <v>46</v>
       </c>
@@ -810,6 +822,9 @@
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Avance en DAG para validadores
Se crean procedimientos de validacion para rdc01 y rdc20, se empieza a trabajar en los DAG del validador
</commit_message>
<xml_diff>
--- a/Analisis/validaciones/validacion_reportes.xlsx
+++ b/Analisis/validaciones/validacion_reportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/validaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="13_ncr:1_{C3BC911C-CB85-46EA-967D-51D15C7D4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{598B92BE-EC3A-4F37-A2D0-6FF2E4D670BF}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{C3BC911C-CB85-46EA-967D-51D15C7D4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{469F7411-3DD0-48C6-9B06-D8721EBFA650}"/>
   <bookViews>
     <workbookView xWindow="13590" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>num_validador</t>
   </si>
@@ -199,6 +199,39 @@
   </si>
   <si>
     <t>proceso.val_en_dominio</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Tipo de registro no corresponde</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Tipo de flujo informado no corresponde</t>
+  </si>
+  <si>
+    <t>RDC20</t>
+  </si>
+  <si>
+    <t>Corresponde a validar si los tipos de registros corresponden a lo solicitado</t>
+  </si>
+  <si>
+    <t>Corresponde a validar el dato que solicita RDC20 para el campo tipo de flujo</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>proceso.val_num_16</t>
+  </si>
+  <si>
+    <t>Filler debe ser completado con espacios y tener un largo especifico</t>
+  </si>
+  <si>
+    <t>Corresponde a validar el filler si esta compuesto por espacios y tiene un largo especifico</t>
   </si>
 </sst>
 </file>
@@ -533,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -830,6 +863,66 @@
         <v>47</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>